<commit_message>
Résultats de la votation inter-communale du 19 mai 2019
</commit_message>
<xml_diff>
--- a/05Resultats/VotationsCOM/2019-05-19_STEP.xlsx
+++ b/05Resultats/VotationsCOM/2019-05-19_STEP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\OneDrive\Documents\GitHub\JuraVote-static\05Resultats\VotationsCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B045E81-6835-4B7D-83F1-0BD0ECE6FE62}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5647D59E-4250-4CCD-9F31-B0015585E163}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1920" windowWidth="29040" windowHeight="16440" xr2:uid="{11934465-9C98-4DE7-9AEF-F7323C33DB8F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Châtillon</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Communes</t>
-  </si>
-  <si>
-    <t>Non disponibles</t>
   </si>
 </sst>
 </file>
@@ -157,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -171,6 +168,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,7 +487,7 @@
   <dimension ref="A4:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +524,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -539,7 +537,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -552,161 +550,143 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="1">
-        <v>790</v>
-      </c>
-      <c r="D7" s="1">
-        <v>114</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" ref="E7:E11" si="0">SUM(C7:D7)</f>
-        <v>904</v>
-      </c>
-      <c r="F7" s="3">
-        <f t="shared" ref="F7:F11" si="1">C7/E7</f>
-        <v>0.87389380530973448</v>
-      </c>
-      <c r="G7" s="3">
-        <f t="shared" ref="G7:G11" si="2">D7/E7</f>
-        <v>0.12610619469026549</v>
-      </c>
-      <c r="H7">
-        <v>37</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1">
-        <v>301</v>
-      </c>
-      <c r="D8" s="1">
-        <v>42</v>
-      </c>
-      <c r="E8" s="2">
-        <f t="shared" si="0"/>
-        <v>343</v>
-      </c>
-      <c r="F8" s="3">
-        <f t="shared" si="1"/>
-        <v>0.87755102040816324</v>
-      </c>
-      <c r="G8" s="3">
-        <f t="shared" si="2"/>
-        <v>0.12244897959183673</v>
-      </c>
-      <c r="H8">
-        <v>33.909999999999997</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="1">
-        <v>1366</v>
+        <v>572</v>
       </c>
       <c r="D9" s="1">
-        <v>351</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="0"/>
-        <v>1717</v>
+        <f>SUM(C9:D9)</f>
+        <v>634</v>
       </c>
       <c r="F9" s="3">
-        <f t="shared" si="1"/>
-        <v>0.79557367501456033</v>
+        <f>C9/E9</f>
+        <v>0.90220820189274453</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="2"/>
-        <v>0.20442632498543972</v>
+        <f>D9/E9</f>
+        <v>9.7791798107255523E-2</v>
       </c>
       <c r="H9">
-        <v>32.9</v>
+        <v>32.6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="1">
-        <v>572</v>
-      </c>
-      <c r="D10" s="1">
-        <v>62</v>
-      </c>
+        <v>2642</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="2">
-        <f t="shared" si="0"/>
-        <v>634</v>
+        <f>SUM(C10:D10)</f>
+        <v>2642</v>
       </c>
       <c r="F10" s="3">
-        <f t="shared" si="1"/>
-        <v>0.90220820189274453</v>
+        <f>C10/E10</f>
+        <v>1</v>
       </c>
       <c r="G10" s="3">
-        <f t="shared" si="2"/>
-        <v>9.7791798107255523E-2</v>
-      </c>
-      <c r="H10">
-        <v>32.6</v>
+        <f>D10/E10</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="1">
-        <v>2642</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>301</v>
+      </c>
+      <c r="D11" s="1">
+        <v>42</v>
+      </c>
       <c r="E11" s="2">
-        <f t="shared" si="0"/>
-        <v>2642</v>
+        <f>SUM(C11:D11)</f>
+        <v>343</v>
       </c>
       <c r="F11" s="3">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>C11/E11</f>
+        <v>0.87755102040816324</v>
       </c>
       <c r="G11" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f>D11/E11</f>
+        <v>0.12244897959183673</v>
+      </c>
+      <c r="H11">
+        <v>33.909999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1366</v>
+      </c>
+      <c r="D12" s="4">
+        <v>351</v>
+      </c>
+      <c r="E12" s="2">
+        <f>SUM(C12:D12)</f>
+        <v>1717</v>
+      </c>
+      <c r="F12" s="3">
+        <f>C12/E12</f>
+        <v>0.79557367501456033</v>
+      </c>
+      <c r="G12" s="3">
+        <f>D12/E12</f>
+        <v>0.20442632498543972</v>
+      </c>
+      <c r="H12">
+        <v>32.9</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>7</v>
@@ -719,7 +699,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>7</v>
@@ -745,7 +725,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>7</v>
@@ -756,9 +736,9 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>7</v>
@@ -769,23 +749,39 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C18" s="1">
+        <v>790</v>
+      </c>
+      <c r="D18" s="1">
+        <v>114</v>
+      </c>
+      <c r="E18" s="2">
+        <f>SUM(C18:D18)</f>
+        <v>904</v>
+      </c>
+      <c r="F18" s="3">
+        <f>C18/E18</f>
+        <v>0.87389380530973448</v>
+      </c>
+      <c r="G18" s="3">
+        <f>D18/E18</f>
+        <v>0.12610619469026549</v>
+      </c>
+      <c r="H18">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B12:H12"/>
-  </mergeCells>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:H18">
+    <sortCondition ref="A5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>